<commit_message>
instrument select operate, remote button start offset button clear
</commit_message>
<xml_diff>
--- a/auto_config.xlsx
+++ b/auto_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC3751E-879D-4A73-BC01-D1C44EEAD118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B78269-027A-41BE-B48E-7775455718E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-56235" yWindow="3225" windowWidth="14010" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25830" yWindow="2235" windowWidth="23325" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -61,10 +61,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GPIB, USB, Serial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,10 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>if select serial, Baudrate data needed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Aging time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -317,6 +309,15 @@
   </si>
   <si>
     <t>atr p out power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIB, USB, Serial, Ethernet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if select serial, Baudrate data needed
+if select ethernet ip address needed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -366,9 +367,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -651,7 +669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -673,63 +693,63 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" t="s">
-        <v>53</v>
-      </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
-        <v>47</v>
-      </c>
       <c r="R1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -741,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -765,22 +785,22 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
@@ -806,13 +826,13 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>18</v>
       </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
       <c r="J3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -821,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="M3">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -850,7 +870,7 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>1.1499999999999999</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
@@ -864,7 +884,7 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>1.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
@@ -878,7 +898,7 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>1.25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
@@ -892,7 +912,7 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>1.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
@@ -906,7 +926,7 @@
         <v>50</v>
       </c>
       <c r="M8">
-        <v>1.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -919,9 +939,6 @@
       <c r="C9">
         <v>50</v>
       </c>
-      <c r="M9">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10">
@@ -933,9 +950,6 @@
       <c r="C10">
         <v>50</v>
       </c>
-      <c r="M10">
-        <v>1.6</v>
-      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11">
@@ -947,9 +961,6 @@
       <c r="C11">
         <v>50</v>
       </c>
-      <c r="M11">
-        <v>1.8</v>
-      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12">
@@ -960,9 +971,6 @@
       </c>
       <c r="C12">
         <v>50</v>
-      </c>
-      <c r="M12">
-        <v>1.99</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
@@ -987,15 +995,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200DA2CE-D9F0-4A24-84A6-96B5876B084D}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
@@ -1003,321 +1011,329 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>43</v>
+      <c r="A1" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="str">
+      <c r="A2" s="4" t="str">
         <f>config!A1</f>
         <v>Frequency</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" t="str">
+      <c r="A3" s="4" t="str">
         <f>config!B1</f>
         <v>Input offset</v>
       </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="str">
+      <c r="A4" s="4" t="str">
         <f>config!C1</f>
         <v>Output offset</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="str">
+      <c r="A5" s="4" t="str">
         <f>config!D1</f>
         <v>Power Voltage</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="str">
+      <c r="A6" s="4" t="str">
         <f>config!E1</f>
         <v>Power Current Limit</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="str">
+      <c r="A7" s="4" t="str">
         <f>config!F1</f>
         <v>Power meter probe Channel</v>
       </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="str">
+      <c r="A8" s="4" t="str">
         <f>config!G1</f>
         <v>Aging time</v>
       </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="str">
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="str">
         <f>config!H1</f>
         <v>Source generate</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="str">
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="str">
         <f>config!I1</f>
         <v>Power supply comm</v>
       </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="str">
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="str">
         <f>config!J1</f>
         <v>Power meter comm</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" t="str">
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="str">
         <f>config!K1</f>
         <v>Spectrum comm</v>
       </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" t="str">
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="str">
         <f>config!L1</f>
         <v>Network comm</v>
       </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" t="str">
+      <c r="A14" s="4" t="str">
         <f>config!M1</f>
         <v>Select Freq</v>
       </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
+      <c r="D14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" t="str">
+      <c r="A15" s="4" t="str">
         <f>config!N1</f>
         <v>Output offset ref power</v>
       </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" t="str">
+      <c r="A16" s="4" t="str">
         <f>config!O1</f>
         <v>ATR start input dBm</v>
       </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="str">
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="str">
         <f>config!P1</f>
         <v>Psat input</v>
       </c>
-      <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="str">
+      <c r="B17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="str">
         <f>config!Q1</f>
         <v>Overdrive input</v>
       </c>
-      <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" t="str">
+      <c r="B18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="str">
         <f>config!R1</f>
         <v>Pout</v>
       </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
power meter remote 외형 구현 offset 구현중
</commit_message>
<xml_diff>
--- a/auto_config.xlsx
+++ b/auto_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B78269-027A-41BE-B48E-7775455718E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B2534-5221-4A9D-BC80-909216C55F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25830" yWindow="2235" windowWidth="23325" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2688" windowWidth="16236" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>dB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -318,6 +318,10 @@
   <si>
     <t>if select serial, Baudrate data needed
 if select ethernet ip address needed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MHz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -667,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="H87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -785,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
         <v>42</v>
@@ -826,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="I3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J3">
         <v>13</v>
@@ -841,10 +845,10 @@
         <v>16</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O3">
         <v>-20</v>
@@ -870,7 +874,7 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
@@ -884,7 +888,11 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <f>M4+$N$5</f>
+        <v>1050</v>
+      </c>
+      <c r="N5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
@@ -898,7 +906,8 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <f t="shared" ref="M6:M69" si="0">M5+$N$5</f>
+        <v>1100</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
@@ -912,7 +921,8 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>1150</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
@@ -926,7 +936,8 @@
         <v>50</v>
       </c>
       <c r="M8">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>1200</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -939,6 +950,10 @@
       <c r="C9">
         <v>50</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10">
@@ -950,6 +965,10 @@
       <c r="C10">
         <v>50</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11">
@@ -961,6 +980,10 @@
       <c r="C11">
         <v>50</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>1350</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12">
@@ -972,6 +995,10 @@
       <c r="C12">
         <v>50</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13">
@@ -982,6 +1009,556 @@
       </c>
       <c r="C13">
         <v>50</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="20" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="21" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="23" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="24" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="26" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="27" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="28" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="29" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="30" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="31" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="32" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M36">
+        <f t="shared" si="0"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M38">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="39" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M39">
+        <f t="shared" si="0"/>
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="40" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M40">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="41" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M41">
+        <f t="shared" si="0"/>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M42">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="44" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M44">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M45">
+        <f t="shared" si="0"/>
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="46" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M46">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M47">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="48" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M48">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M50">
+        <f t="shared" si="0"/>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M51">
+        <f t="shared" si="0"/>
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M52">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M53">
+        <f t="shared" si="0"/>
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M54">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M55">
+        <f t="shared" si="0"/>
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M56">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M57">
+        <f t="shared" si="0"/>
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="58" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M58">
+        <f t="shared" si="0"/>
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="59" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M59">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="60" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M60">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="61" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M61">
+        <f t="shared" si="0"/>
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="62" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M62">
+        <f t="shared" si="0"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="63" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M63">
+        <f t="shared" si="0"/>
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="64" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M64">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="65" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M65">
+        <f t="shared" si="0"/>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="66" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M66">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="67" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M67">
+        <f t="shared" si="0"/>
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="68" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M68">
+        <f t="shared" si="0"/>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="69" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M69">
+        <f t="shared" si="0"/>
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="70" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M70">
+        <f t="shared" ref="M70:M122" si="1">M69+$N$5</f>
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="71" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M71">
+        <f t="shared" si="1"/>
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="72" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M72">
+        <f t="shared" si="1"/>
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="73" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M73">
+        <f t="shared" si="1"/>
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="74" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M74">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="75" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M75">
+        <f t="shared" si="1"/>
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="76" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M76">
+        <f t="shared" si="1"/>
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="77" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M77">
+        <f t="shared" si="1"/>
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="78" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M78">
+        <f t="shared" si="1"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="79" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M79">
+        <f t="shared" si="1"/>
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="80" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M80">
+        <f t="shared" si="1"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M81">
+        <f t="shared" si="1"/>
+        <v>4850</v>
+      </c>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M82">
+        <f t="shared" si="1"/>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M83">
+        <f t="shared" si="1"/>
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M84">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M85">
+        <f t="shared" si="1"/>
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M86">
+        <f t="shared" si="1"/>
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="87" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M87">
+        <f t="shared" si="1"/>
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="88" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M88">
+        <f t="shared" si="1"/>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="89" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M89">
+        <f t="shared" si="1"/>
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="90" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M90">
+        <f t="shared" si="1"/>
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="91" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M91">
+        <f t="shared" si="1"/>
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="92" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M92">
+        <f t="shared" si="1"/>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="93" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M93">
+        <f t="shared" si="1"/>
+        <v>5450</v>
+      </c>
+    </row>
+    <row r="94" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M94">
+        <f t="shared" si="1"/>
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="95" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M95">
+        <f t="shared" si="1"/>
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="96" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M96">
+        <f t="shared" si="1"/>
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M97">
+        <f t="shared" si="1"/>
+        <v>5650</v>
+      </c>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M98">
+        <f t="shared" si="1"/>
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="99" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M99">
+        <f t="shared" si="1"/>
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="100" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M100">
+        <f t="shared" si="1"/>
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="101" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M101">
+        <f t="shared" si="1"/>
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="102" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M102">
+        <f t="shared" si="1"/>
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="103" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M103">
+        <f t="shared" si="1"/>
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="104" spans="13:13" x14ac:dyDescent="0.4">
+      <c r="M104">
+        <f t="shared" si="1"/>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>